<commit_message>
Reporte de avance en programas
</commit_message>
<xml_diff>
--- a/docs/formatos/avanceProgramas.xlsx
+++ b/docs/formatos/avanceProgramas.xlsx
@@ -85,7 +85,7 @@
     <t>Hora Fin</t>
   </si>
   <si>
-    <t>Fecha InFin</t>
+    <t>Fecha Fin</t>
   </si>
 </sst>
 </file>
@@ -233,19 +233,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,46 +557,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15"/>
-    </row>
-    <row r="2" spans="1:19" s="18" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="15"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="18"/>
+    </row>
+    <row r="2" spans="1:19" s="16" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -662,16 +662,16 @@
       <c r="N4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="R4" s="14" t="s">
         <v>18</v>
       </c>
       <c r="S4" s="4" t="s">
@@ -693,7 +693,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="17"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="7"/>

</xml_diff>

<commit_message>
avance en programas y conexiones por usuario con incidencias resueltas
</commit_message>
<xml_diff>
--- a/docs/formatos/avanceProgramas.xlsx
+++ b/docs/formatos/avanceProgramas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Usuario</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Fecha Fin</t>
+  </si>
+  <si>
+    <t>Estatus del programa</t>
   </si>
 </sst>
 </file>
@@ -150,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,12 +196,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -245,6 +259,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -527,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,9 +577,10 @@
     <col min="17" max="17" width="27.140625" customWidth="1"/>
     <col min="18" max="18" width="26.42578125" customWidth="1"/>
     <col min="19" max="19" width="23.28515625" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -577,7 +601,7 @@
       <c r="R1" s="17"/>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:19" s="16" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="16" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -598,7 +622,7 @@
       <c r="R2" s="17"/>
       <c r="S2" s="18"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -619,7 +643,7 @@
       <c r="R3" s="10"/>
       <c r="S3" s="9"/>
     </row>
-    <row r="4" spans="1:19" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -666,19 +690,22 @@
         <v>14</v>
       </c>
       <c r="P4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="S4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -698,20 +725,25 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="21"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G10" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes en reportes backend
</commit_message>
<xml_diff>
--- a/docs/formatos/avanceProgramas.xlsx
+++ b/docs/formatos/avanceProgramas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\formacion2.0\docs\formatos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="USUARIOS_20150209" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -94,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,16 +126,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -244,30 +237,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -330,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,7 +358,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,46 +574,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="18"/>
-    </row>
-    <row r="2" spans="1:20" s="16" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="18"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="20"/>
+    </row>
+    <row r="2" spans="1:20" s="15" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -686,19 +679,19 @@
       <c r="N4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="T4" s="4" t="s">
@@ -711,7 +704,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -720,19 +713,19 @@
       <c r="L5" s="6"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="15"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-      <c r="T5" s="21"/>
+      <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G6" s="12"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="20"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="18"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G7" s="12"/>

</xml_diff>

<commit_message>
montando ajustes en master
</commit_message>
<xml_diff>
--- a/docs/formatos/avanceProgramas.xlsx
+++ b/docs/formatos/avanceProgramas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\formacion2.0\docs\formatos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,17 +17,20 @@
   <definedNames>
     <definedName name="USUARIOS_20150209" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Código</t>
+  </si>
   <si>
     <t>Usuario</t>
   </si>
@@ -33,6 +41,15 @@
     <t>Apellido</t>
   </si>
   <si>
+    <t>Fecha de Registro</t>
+  </si>
+  <si>
+    <t>Hora de registro</t>
+  </si>
+  <si>
+    <t>Acceso</t>
+  </si>
+  <si>
     <t>Correo</t>
   </si>
   <si>
@@ -52,12 +69,6 @@
   </si>
   <si>
     <t>Campo4</t>
-  </si>
-  <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>Fecha de Registro</t>
   </si>
   <si>
     <t xml:space="preserve">Módulos Vistos
@@ -71,77 +82,82 @@
     <t>Promedio Evaluación Módulo</t>
   </si>
   <si>
+    <t>Estatus del programa</t>
+  </si>
+  <si>
     <t>Fecha Inicio</t>
   </si>
   <si>
     <t>Hora Inicio</t>
   </si>
   <si>
+    <t>Fecha Fin</t>
+  </si>
+  <si>
     <t>Hora Fin</t>
   </si>
   <si>
-    <t>Fecha Fin</t>
-  </si>
-  <si>
-    <t>Estatus del programa</t>
-  </si>
-  <si>
-    <t>Acceso</t>
-  </si>
-  <si>
-    <t>Hora de registro</t>
+    <t>Tiempo total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="hh:mm"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,24 +177,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -187,78 +188,92 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -267,6 +282,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0563C1"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -321,12 +404,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -356,12 +439,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -533,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,13 +624,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
@@ -571,188 +654,193 @@
     <col min="20" max="20" width="23.42578125" customWidth="1"/>
     <col min="21" max="21" width="15.7109375" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="22"/>
-    </row>
-    <row r="2" spans="1:22" s="15" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="22"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="9"/>
-    </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="L4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="M4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="19"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="G6" s="12"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="G10" s="12"/>
+      <c r="W4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="17" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G6" s="18"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G10" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajuste en el formato excel de avanceprogramas
</commit_message>
<xml_diff>
--- a/docs/formatos/avanceProgramas.xlsx
+++ b/docs/formatos/avanceProgramas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\formacion2.0\docs\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902C1249-5F50-456F-A642-E8121763D002}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -97,16 +98,16 @@
     <t>Hora Fin</t>
   </si>
   <si>
-    <t>Tiempo total</t>
-  </si>
-  <si>
     <t>Logueado</t>
+  </si>
+  <si>
+    <t>Tiempo acumulado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm"/>
   </numFmts>
@@ -626,11 +627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>7</v>
@@ -797,7 +798,7 @@
         <v>21</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>